<commit_message>
Fix test template. Remove propertyvalues tied to removed propertytypes.
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Experiment_run_Infinium_v5_0_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Experiment_run_Infinium_v5_0_0.xlsx
@@ -2202,7 +2202,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.43"/>
@@ -44355,7 +44355,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="24.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.86"/>
@@ -44446,6 +44446,9 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="23"/>
+      <c r="F5" s="1" t="n">
+        <v>29</v>
+      </c>
       <c r="G5" s="3" t="s">
         <v>99</v>
       </c>
@@ -52229,7 +52232,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.43"/>

</xml_diff>